<commit_message>
add regulator, BOM, schematic, layout updates
</commit_message>
<xml_diff>
--- a/hardware/Console_Lights_BOM.xlsx
+++ b/hardware/Console_Lights_BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="109">
   <si>
     <t xml:space="preserve">Console Lights PCBA BOM v0.1</t>
   </si>
@@ -125,7 +125,28 @@
     <t xml:space="preserve">ULN2003V12T16-13</t>
   </si>
   <si>
-    <t xml:space="preserve">D201, D203</t>
+    <t xml:space="preserve">U106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Semi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCP1117DT50RKG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V Linear Regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.onsemi.com/pub/Collateral/NCP1117-D.PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.arrow.com/en/products/ncp1117dt50rkg/on-semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en/integrated-circuits-ics/pmic-voltage-regulators-linear/699?k=NCP1117&amp;k=&amp;pkeyword=NCP1117&amp;pv1291=6351&amp;sf=0&amp;FV=1c0002%2Ca4027c%2C1f140000%2Cffe002bb%2C1bcc0038&amp;quantity=&amp;ColumnSort=0&amp;page=1&amp;pageSize=25</t>
   </si>
   <si>
     <t xml:space="preserve">J501</t>
@@ -197,9 +218,6 @@
     <t xml:space="preserve">http://www.farnell.com/datasheets/5448.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">RN701,RN702</t>
-  </si>
-  <si>
     <t xml:space="preserve">R703</t>
   </si>
   <si>
@@ -209,19 +227,40 @@
     <t xml:space="preserve">R702</t>
   </si>
   <si>
-    <t xml:space="preserve">R705, R706</t>
-  </si>
-  <si>
     <t xml:space="preserve">R701</t>
   </si>
   <si>
-    <t xml:space="preserve">C805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C806</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C801, C802, C803, C804</t>
+    <t xml:space="preserve">C801, C802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1uF Capacitor, +/-10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pansonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVQ-Q2K01W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tactile Switch, SPST-NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://industrial.panasonic.com/ac/cdn/e/control/switch/light-touch/catalog/sw_lt_eng_6s_th.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.arrow.com/en/products/evq-q2k01w/panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en/switches/tactile-switches/197?k=EVQ-Q2K01W&amp;k=&amp;pkeyword=EVQ-Q2K01W&amp;pv7=2&amp;mnonly=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVQ-Q2P02W, EVQ-Q2P03W, EVQ-Q2K03W</t>
   </si>
   <si>
     <t xml:space="preserve">Console Lights Other</t>
@@ -452,7 +491,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -518,6 +557,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,7 +646,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -611,19 +654,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="46.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="1021" min="12" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -768,122 +811,138 @@
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="0"/>
@@ -896,94 +955,80 @@
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>2</v>
+      </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-    </row>
-    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -999,14 +1044,20 @@
     <hyperlink ref="G5" r:id="rId7" display="http://www.ti.com/lit/ds/symlink/uln2003a.pdf"/>
     <hyperlink ref="H5" r:id="rId8" display="https://www.arrow.com/en/products/uln2003apwr/texas-instruments"/>
     <hyperlink ref="I5" r:id="rId9" display="https://www.digikey.com/product-detail/en/texas-instruments/ULN2003APWR/296-27173-1-ND/2255408"/>
-    <hyperlink ref="G7" r:id="rId10" display="https://www.andersonpower.com/_global-assets/downloads/pdf/b02021s.pdf"/>
-    <hyperlink ref="H7" r:id="rId11" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/ASMPR45-1X2-RK?qs=tub3WQyKOl%2FsXEao4JOdAw%3D%3D"/>
-    <hyperlink ref="G8" r:id="rId12" display="https://drawings-pdf.s3.amazonaws.com/10492.pdf"/>
-    <hyperlink ref="H8" r:id="rId13" display="https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC141LFBN-RC/S7047-ND/810186"/>
-    <hyperlink ref="G9" r:id="rId14" display="http://www.jst-mfg.com/product/pdf/eng/eXH.pdf"/>
-    <hyperlink ref="H9" r:id="rId15" display="https://www.arrow.com/en/products/s4b-xh-sm4-tb-lf-sn/jst-manufacturing"/>
-    <hyperlink ref="I9" r:id="rId16" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S4B-XH-SM4-TB-LF-SN/455-2262-1-ND/1651060"/>
-    <hyperlink ref="J9" r:id="rId17" display="http://www.farnell.com/datasheets/5448.pdf"/>
+    <hyperlink ref="G6" r:id="rId10" display="http://www.onsemi.com/pub/Collateral/NCP1117-D.PDF"/>
+    <hyperlink ref="H6" r:id="rId11" display="https://www.arrow.com/en/products/ncp1117dt50rkg/on-semiconductor"/>
+    <hyperlink ref="I6" r:id="rId12" display="https://www.digikey.com/products/en/integrated-circuits-ics/pmic-voltage-regulators-linear/699?k=NCP1117&amp;k=&amp;pkeyword=NCP1117&amp;pv1291=6351&amp;sf=0&amp;FV=1c0002%2Ca4027c%2C1f140000%2Cffe002bb%2C1bcc0038&amp;quantity=&amp;ColumnSort=0&amp;page=1&amp;pageSize=25"/>
+    <hyperlink ref="G7" r:id="rId13" display="https://www.andersonpower.com/_global-assets/downloads/pdf/b02021s.pdf"/>
+    <hyperlink ref="H7" r:id="rId14" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/ASMPR45-1X2-RK?qs=tub3WQyKOl%2FsXEao4JOdAw%3D%3D"/>
+    <hyperlink ref="G8" r:id="rId15" display="https://drawings-pdf.s3.amazonaws.com/10492.pdf"/>
+    <hyperlink ref="H8" r:id="rId16" display="https://www.digikey.com/product-detail/en/sullins-connector-solutions/PPPC141LFBN-RC/S7047-ND/810186"/>
+    <hyperlink ref="G9" r:id="rId17" display="http://www.jst-mfg.com/product/pdf/eng/eXH.pdf"/>
+    <hyperlink ref="H9" r:id="rId18" display="https://www.arrow.com/en/products/s4b-xh-sm4-tb-lf-sn/jst-manufacturing"/>
+    <hyperlink ref="I9" r:id="rId19" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/S4B-XH-SM4-TB-LF-SN/455-2262-1-ND/1651060"/>
+    <hyperlink ref="J9" r:id="rId20" display="http://www.farnell.com/datasheets/5448.pdf"/>
+    <hyperlink ref="G15" r:id="rId21" display="https://industrial.panasonic.com/ac/cdn/e/control/switch/light-touch/catalog/sw_lt_eng_6s_th.pdf"/>
+    <hyperlink ref="H15" r:id="rId22" display="https://www.arrow.com/en/products/evq-q2k01w/panasonic"/>
+    <hyperlink ref="I15" r:id="rId23" display="https://www.digikey.com/products/en/switches/tactile-switches/197?k=EVQ-Q2K01W&amp;k=&amp;pkeyword=EVQ-Q2K01W&amp;pv7=2&amp;mnonly=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.02638888888889" bottom="1.02638888888889" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1031,21 +1082,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.29081632653061"/>
     <col collapsed="false" hidden="false" max="1018" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="7.1530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1082,22 +1133,22 @@
         <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1105,22 +1156,22 @@
         <v>10</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,126 +1179,126 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="17"/>
+        <v>90</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G6" s="17"/>
+        <v>94</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="17"/>
+        <v>97</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="17"/>
+        <v>101</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G9" s="17"/>
+        <v>104</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="17"/>
+        <v>107</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add quick-connects to BOM
</commit_message>
<xml_diff>
--- a/hardware/Console_Lights_BOM.xlsx
+++ b/hardware/Console_Lights_BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="120">
   <si>
     <t xml:space="preserve">Console Lights PCBA BOM v0.1</t>
   </si>
@@ -294,6 +294,33 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/product-detail/en/jst-sales-america-inc/XHP-4/455-2267-ND/683353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62094-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn Quick Connect 0.110 x 0.020 Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=62094&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/62094-1/A27751CT-ND/456839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60118-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conn Quick Connect 0.110 x 0.016 Tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=60118&amp;DocType=Customer+Drawing&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/60118-1/A27748CT-ND/456836</t>
   </si>
   <si>
     <t xml:space="preserve">1399G8-BK</t>
@@ -634,25 +661,24 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.8214285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="46.4030612244898"/>
     <col collapsed="false" hidden="false" max="1021" min="12" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1030,7 +1056,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1038,16 +1064,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.47959183673469"/>
     <col collapsed="false" hidden="false" max="1018" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1130,108 +1156,108 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="C5" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="18"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="E6" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="F8" s="18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>101</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G9" s="18"/>
     </row>
@@ -1240,21 +1266,63 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E10" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="C11" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="18"/>
+      <c r="C12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G12" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1267,18 +1335,22 @@
     <hyperlink ref="E4" r:id="rId4" display="http://www.jst-mfg.com/product/pdf/eng/eXH.pdf"/>
     <hyperlink ref="F4" r:id="rId5" display="https://www.arrow.com/en/products/xhp-4/jst-manufacturing"/>
     <hyperlink ref="G4" r:id="rId6" display="https://www.digikey.com/product-detail/en/jst-sales-america-inc/XHP-4/455-2267-ND/683353"/>
-    <hyperlink ref="E5" r:id="rId7" display="https://www.mouser.com/datasheet/2/22/AndersonPower_01102017_DS-PP1545-1158138.pdf"/>
-    <hyperlink ref="F5" r:id="rId8" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/1399G8-BK?qs=%2Fha2pyFaduh5jUyI6iXVHVzwlETYCyYS1Ae5gHXLiNw%3D"/>
-    <hyperlink ref="E6" r:id="rId9" display="https://www.mouser.com/datasheet/2/22/AndersonPower_01102017_DS-PP1545-1158138.pdf"/>
-    <hyperlink ref="F6" r:id="rId10" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/110G16?qs=sGAEpiMZZMvlX3nhDDO4ALNZHDn%2FFYPdkeo8iDYdwBE%3D"/>
-    <hyperlink ref="E7" r:id="rId11" display="https://www.andersonpower.com/_global-assets/downloads/pdf/b02021s.pdf"/>
-    <hyperlink ref="F7" r:id="rId12" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/114555P2?qs=%2Fha2pyFadujeSQxJp0HvYijPO3yM9ImmDwlzJH6kvKU%3D"/>
-    <hyperlink ref="E8" r:id="rId13" display="https://www.mcmaster.com/91290a383"/>
-    <hyperlink ref="F8" r:id="rId14" display="https://www.mcmaster.com/91290a383"/>
-    <hyperlink ref="E9" r:id="rId15" display="https://www.mcmaster.com/94150a330"/>
-    <hyperlink ref="F9" r:id="rId16" display="https://www.mcmaster.com/94150a330"/>
-    <hyperlink ref="E10" r:id="rId17" display="https://www.mcmaster.com/90965a140"/>
-    <hyperlink ref="F10" r:id="rId18" display="https://www.mcmaster.com/90965a140"/>
+    <hyperlink ref="E5" r:id="rId7" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=62094&amp;DocType=Customer+Drawing&amp;DocLang=English"/>
+    <hyperlink ref="F5" r:id="rId8" display="https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/62094-1/A27751CT-ND/456839"/>
+    <hyperlink ref="E6" r:id="rId9" display="https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=60118&amp;DocType=Customer+Drawing&amp;DocLang=English"/>
+    <hyperlink ref="F6" r:id="rId10" display="https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/60118-1/A27748CT-ND/456836"/>
+    <hyperlink ref="E7" r:id="rId11" display="https://www.mouser.com/datasheet/2/22/AndersonPower_01102017_DS-PP1545-1158138.pdf"/>
+    <hyperlink ref="F7" r:id="rId12" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/1399G8-BK?qs=%2Fha2pyFaduh5jUyI6iXVHVzwlETYCyYS1Ae5gHXLiNw%3D"/>
+    <hyperlink ref="E8" r:id="rId13" display="https://www.mouser.com/datasheet/2/22/AndersonPower_01102017_DS-PP1545-1158138.pdf"/>
+    <hyperlink ref="F8" r:id="rId14" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/110G16?qs=sGAEpiMZZMvlX3nhDDO4ALNZHDn%2FFYPdkeo8iDYdwBE%3D"/>
+    <hyperlink ref="E9" r:id="rId15" display="https://www.andersonpower.com/_global-assets/downloads/pdf/b02021s.pdf"/>
+    <hyperlink ref="F9" r:id="rId16" display="https://www.mouser.com/ProductDetail/Anderson-Power-Products/114555P2?qs=%2Fha2pyFadujeSQxJp0HvYijPO3yM9ImmDwlzJH6kvKU%3D"/>
+    <hyperlink ref="E10" r:id="rId17" display="https://www.mcmaster.com/91290a383"/>
+    <hyperlink ref="F10" r:id="rId18" display="https://www.mcmaster.com/91290a383"/>
+    <hyperlink ref="E11" r:id="rId19" display="https://www.mcmaster.com/94150a330"/>
+    <hyperlink ref="F11" r:id="rId20" display="https://www.mcmaster.com/94150a330"/>
+    <hyperlink ref="E12" r:id="rId21" display="https://www.mcmaster.com/90965a140"/>
+    <hyperlink ref="F12" r:id="rId22" display="https://www.mcmaster.com/90965a140"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>